<commit_message>
run some of the 27 and 31 degree TA
</commit_message>
<xml_diff>
--- a/Data/BermudaSalinity.xlsx
+++ b/Data/BermudaSalinity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="340">
   <si>
     <t>Fragment.ID</t>
   </si>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="B288" workbookViewId="0">
+      <selection activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,7 +3767,7 @@
         <v>37.380000000000003</v>
       </c>
       <c r="D203" s="4">
-        <v>43185</v>
+        <v>43187</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>339</v>
@@ -3780,9 +3780,15 @@
       <c r="B204" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C204" s="2"/>
-      <c r="D204" s="1"/>
-      <c r="E204" s="1"/>
+      <c r="C204" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D204" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
@@ -4666,9 +4672,15 @@
       <c r="B284" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C284" s="2"/>
-      <c r="D284" s="1"/>
-      <c r="E284" s="1"/>
+      <c r="C284" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D284" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
@@ -4677,9 +4689,15 @@
       <c r="B285" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C285" s="2"/>
-      <c r="D285" s="1"/>
-      <c r="E285" s="1"/>
+      <c r="C285" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D285" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
@@ -4688,9 +4706,15 @@
       <c r="B286" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C286" s="2"/>
-      <c r="D286" s="1"/>
-      <c r="E286" s="1"/>
+      <c r="C286" s="2">
+        <v>37.79</v>
+      </c>
+      <c r="D286" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
@@ -4699,9 +4723,15 @@
       <c r="B287" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C287" s="2"/>
-      <c r="D287" s="1"/>
-      <c r="E287" s="1"/>
+      <c r="C287" s="2">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="D287" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
@@ -4721,9 +4751,15 @@
       <c r="B289" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C289" s="2"/>
-      <c r="D289" s="1"/>
-      <c r="E289" s="1"/>
+      <c r="C289" s="2">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="D289" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
@@ -4732,9 +4768,15 @@
       <c r="B290" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C290" s="2"/>
-      <c r="D290" s="1"/>
-      <c r="E290" s="1"/>
+      <c r="C290" s="2">
+        <v>37.75</v>
+      </c>
+      <c r="D290" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
@@ -4743,9 +4785,15 @@
       <c r="B291" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C291" s="2"/>
-      <c r="D291" s="1"/>
-      <c r="E291" s="1"/>
+      <c r="C291" s="2">
+        <v>37.75</v>
+      </c>
+      <c r="D291" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
@@ -4754,9 +4802,15 @@
       <c r="B292" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C292" s="2"/>
-      <c r="D292" s="1"/>
-      <c r="E292" s="1"/>
+      <c r="C292" s="2">
+        <v>37.78</v>
+      </c>
+      <c r="D292" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
@@ -4776,9 +4830,15 @@
       <c r="B294" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C294" s="2"/>
-      <c r="D294" s="1"/>
-      <c r="E294" s="1"/>
+      <c r="C294" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D294" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
@@ -4787,9 +4847,15 @@
       <c r="B295" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C295" s="2"/>
-      <c r="D295" s="1"/>
-      <c r="E295" s="1"/>
+      <c r="C295" s="2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D295" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
@@ -4809,9 +4875,15 @@
       <c r="B297" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C297" s="2"/>
-      <c r="D297" s="1"/>
-      <c r="E297" s="1"/>
+      <c r="C297" s="2">
+        <v>37.75</v>
+      </c>
+      <c r="D297" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
@@ -4820,9 +4892,15 @@
       <c r="B298" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C298" s="2"/>
-      <c r="D298" s="1"/>
-      <c r="E298" s="1"/>
+      <c r="C298" s="2">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D298" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
@@ -4842,9 +4920,15 @@
       <c r="B300" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C300" s="2"/>
-      <c r="D300" s="1"/>
-      <c r="E300" s="1"/>
+      <c r="C300" s="2">
+        <v>37.61</v>
+      </c>
+      <c r="D300" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
@@ -4875,9 +4959,15 @@
       <c r="B303" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C303" s="2"/>
-      <c r="D303" s="1"/>
-      <c r="E303" s="1"/>
+      <c r="C303" s="2">
+        <v>37.659999999999997</v>
+      </c>
+      <c r="D303" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
@@ -4886,9 +4976,15 @@
       <c r="B304" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C304" s="2"/>
-      <c r="D304" s="1"/>
-      <c r="E304" s="1"/>
+      <c r="C304" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D304" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
@@ -4897,9 +4993,15 @@
       <c r="B305" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C305" s="2"/>
-      <c r="D305" s="1"/>
-      <c r="E305" s="1"/>
+      <c r="C305" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D305" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
@@ -4908,9 +5010,15 @@
       <c r="B306" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C306" s="2"/>
-      <c r="D306" s="1"/>
-      <c r="E306" s="1"/>
+      <c r="C306" s="2">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="D306" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
@@ -4919,9 +5027,15 @@
       <c r="B307" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C307" s="2"/>
-      <c r="D307" s="1"/>
-      <c r="E307" s="1"/>
+      <c r="C307" s="2">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="D307" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
@@ -4930,9 +5044,15 @@
       <c r="B308" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C308" s="2"/>
-      <c r="D308" s="1"/>
-      <c r="E308" s="1"/>
+      <c r="C308" s="2">
+        <v>37.68</v>
+      </c>
+      <c r="D308" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
@@ -4941,9 +5061,15 @@
       <c r="B309" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C309" s="2"/>
-      <c r="D309" s="1"/>
-      <c r="E309" s="1"/>
+      <c r="C309" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D309" s="4">
+        <v>43187</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="2">

</xml_diff>

<commit_message>
added TA samples from 27 and 29 deg
</commit_message>
<xml_diff>
--- a/Data/BermudaSalinity.xlsx
+++ b/Data/BermudaSalinity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="341">
   <si>
     <t>Fragment.ID</t>
   </si>
@@ -1044,6 +1044,9 @@
   </si>
   <si>
     <t>JM</t>
+  </si>
+  <si>
+    <t>3/39/2018</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B288" workbookViewId="0">
-      <selection activeCell="C306" sqref="C306"/>
+    <sheetView tabSelected="1" topLeftCell="B204" workbookViewId="0">
+      <selection activeCell="C232" sqref="C232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,9 +3817,15 @@
       <c r="B206" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C206" s="2"/>
-      <c r="D206" s="1"/>
-      <c r="E206" s="1"/>
+      <c r="C206" s="2">
+        <v>37.6</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
@@ -3825,9 +3834,15 @@
       <c r="B207" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C207" s="2"/>
-      <c r="D207" s="1"/>
-      <c r="E207" s="1"/>
+      <c r="C207" s="2">
+        <v>37.61</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
@@ -3847,9 +3862,15 @@
       <c r="B209" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C209" s="2"/>
-      <c r="D209" s="1"/>
-      <c r="E209" s="1"/>
+      <c r="C209" s="2">
+        <v>37.65</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
@@ -3858,9 +3879,15 @@
       <c r="B210" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C210" s="2"/>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
+      <c r="C210" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
@@ -3869,9 +3896,15 @@
       <c r="B211" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C211" s="2"/>
-      <c r="D211" s="1"/>
-      <c r="E211" s="1"/>
+      <c r="C211" s="2">
+        <v>37.65</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
@@ -3891,9 +3924,15 @@
       <c r="B213" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C213" s="2"/>
-      <c r="D213" s="1"/>
-      <c r="E213" s="1"/>
+      <c r="C213" s="2">
+        <v>37.619999999999997</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
@@ -3935,9 +3974,15 @@
       <c r="B217" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C217" s="2"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
+      <c r="C217" s="2">
+        <v>37.61</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
@@ -3946,9 +3991,15 @@
       <c r="B218" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C218" s="2"/>
-      <c r="D218" s="1"/>
-      <c r="E218" s="1"/>
+      <c r="C218" s="2">
+        <v>37.65</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
@@ -3968,9 +4019,15 @@
       <c r="B220" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C220" s="2"/>
-      <c r="D220" s="1"/>
-      <c r="E220" s="1"/>
+      <c r="C220" s="2">
+        <v>37.69</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
@@ -3979,9 +4036,15 @@
       <c r="B221" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C221" s="2"/>
-      <c r="D221" s="1"/>
-      <c r="E221" s="1"/>
+      <c r="C221" s="2">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
@@ -3990,9 +4053,15 @@
       <c r="B222" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C222" s="2"/>
-      <c r="D222" s="1"/>
-      <c r="E222" s="1"/>
+      <c r="C222" s="2">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
@@ -4034,9 +4103,15 @@
       <c r="B226" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C226" s="2"/>
-      <c r="D226" s="1"/>
-      <c r="E226" s="1"/>
+      <c r="C226" s="2">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
@@ -4045,9 +4120,15 @@
       <c r="B227" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C227" s="2"/>
-      <c r="D227" s="1"/>
-      <c r="E227" s="1"/>
+      <c r="C227" s="2">
+        <v>37.64</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
@@ -4056,9 +4137,15 @@
       <c r="B228" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C228" s="2"/>
-      <c r="D228" s="1"/>
-      <c r="E228" s="1"/>
+      <c r="C228" s="2">
+        <v>37.71</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
@@ -4067,9 +4154,15 @@
       <c r="B229" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C229" s="2"/>
-      <c r="D229" s="1"/>
-      <c r="E229" s="1"/>
+      <c r="C229" s="2">
+        <v>37.71</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
@@ -4078,9 +4171,15 @@
       <c r="B230" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C230" s="2"/>
-      <c r="D230" s="1"/>
-      <c r="E230" s="1"/>
+      <c r="C230" s="2">
+        <v>37.72</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
@@ -4089,9 +4188,15 @@
       <c r="B231" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C231" s="2"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="1"/>
+      <c r="C231" s="2">
+        <v>37.67</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
@@ -4909,7 +5014,9 @@
       <c r="B299" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C299" s="2"/>
+      <c r="C299" s="2">
+        <v>37.9</v>
+      </c>
       <c r="D299" s="1"/>
       <c r="E299" s="1"/>
     </row>
@@ -5425,6 +5532,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
samples from 24 to 29 degrees added
</commit_message>
<xml_diff>
--- a/Data/BermudaSalinity.xlsx
+++ b/Data/BermudaSalinity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="340">
   <si>
     <t>Fragment.ID</t>
   </si>
@@ -1044,9 +1044,6 @@
   </si>
   <si>
     <t>JM</t>
-  </si>
-  <si>
-    <t>3/39/2018</t>
   </si>
 </sst>
 </file>
@@ -1105,12 +1102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1393,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B204" workbookViewId="0">
-      <selection activeCell="C232" sqref="C232"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="G212" sqref="G212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,9 +1801,15 @@
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="C36" s="2">
+        <v>37.950000000000003</v>
+      </c>
+      <c r="D36" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -1814,9 +1818,15 @@
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="C37" s="2">
+        <v>37.950000000000003</v>
+      </c>
+      <c r="D37" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
@@ -1825,9 +1835,15 @@
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="C38" s="2">
+        <v>37.94</v>
+      </c>
+      <c r="D38" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
@@ -1847,9 +1863,15 @@
       <c r="B40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="C40" s="2">
+        <v>37.96</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -1858,9 +1880,15 @@
       <c r="B41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="C41" s="2">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="D41" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -1880,9 +1908,15 @@
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="C43" s="2">
+        <v>37.92</v>
+      </c>
+      <c r="D43" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -1891,9 +1925,15 @@
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="C44" s="2">
+        <v>37.96</v>
+      </c>
+      <c r="D44" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -1913,9 +1953,15 @@
       <c r="B46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="C46" s="2">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="D46" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -1924,9 +1970,15 @@
       <c r="B47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="C47" s="2">
+        <v>37.94</v>
+      </c>
+      <c r="D47" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -1946,9 +1998,15 @@
       <c r="B49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="C49" s="2">
+        <v>37.96</v>
+      </c>
+      <c r="D49" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -1957,9 +2015,15 @@
       <c r="B50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="C50" s="2">
+        <v>37.93</v>
+      </c>
+      <c r="D50" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -1968,9 +2032,15 @@
       <c r="B51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="C51" s="2">
+        <v>37.96</v>
+      </c>
+      <c r="D51" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -1979,9 +2049,15 @@
       <c r="B52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="C52" s="2">
+        <v>37.93</v>
+      </c>
+      <c r="D52" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -3820,8 +3896,8 @@
       <c r="C206" s="2">
         <v>37.6</v>
       </c>
-      <c r="D206" s="1" t="s">
-        <v>340</v>
+      <c r="D206" s="4">
+        <v>43188</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>339</v>
@@ -3837,8 +3913,8 @@
       <c r="C207" s="2">
         <v>37.61</v>
       </c>
-      <c r="D207" s="1" t="s">
-        <v>340</v>
+      <c r="D207" s="4">
+        <v>43188</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>339</v>
@@ -3851,9 +3927,15 @@
       <c r="B208" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C208" s="2"/>
-      <c r="D208" s="1"/>
-      <c r="E208" s="1"/>
+      <c r="C208" s="2">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="D208" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
@@ -3865,8 +3947,8 @@
       <c r="C209" s="2">
         <v>37.65</v>
       </c>
-      <c r="D209" s="1" t="s">
-        <v>340</v>
+      <c r="D209" s="4">
+        <v>43188</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>339</v>
@@ -3882,8 +3964,8 @@
       <c r="C210" s="2">
         <v>37.64</v>
       </c>
-      <c r="D210" s="1" t="s">
-        <v>340</v>
+      <c r="D210" s="4">
+        <v>43188</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>339</v>
@@ -3897,10 +3979,10 @@
         <v>209</v>
       </c>
       <c r="C211" s="2">
-        <v>37.65</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>340</v>
+        <v>37.72</v>
+      </c>
+      <c r="D211" s="4">
+        <v>43192</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>339</v>
@@ -3913,9 +3995,15 @@
       <c r="B212" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C212" s="2"/>
-      <c r="D212" s="1"/>
-      <c r="E212" s="1"/>
+      <c r="C212" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D212" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
@@ -3927,8 +4015,8 @@
       <c r="C213" s="2">
         <v>37.619999999999997</v>
       </c>
-      <c r="D213" s="1" t="s">
-        <v>340</v>
+      <c r="D213" s="4">
+        <v>43188</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>339</v>
@@ -3941,9 +4029,15 @@
       <c r="B214" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C214" s="2"/>
-      <c r="D214" s="1"/>
-      <c r="E214" s="1"/>
+      <c r="C214" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D214" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
@@ -3952,9 +4046,15 @@
       <c r="B215" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C215" s="2"/>
-      <c r="D215" s="1"/>
-      <c r="E215" s="1"/>
+      <c r="C215" s="2">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D215" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
@@ -3977,8 +4077,8 @@
       <c r="C217" s="2">
         <v>37.61</v>
       </c>
-      <c r="D217" s="1" t="s">
-        <v>340</v>
+      <c r="D217" s="4">
+        <v>43188</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>339</v>
@@ -3994,8 +4094,8 @@
       <c r="C218" s="2">
         <v>37.65</v>
       </c>
-      <c r="D218" s="1" t="s">
-        <v>340</v>
+      <c r="D218" s="4">
+        <v>43188</v>
       </c>
       <c r="E218" s="1" t="s">
         <v>339</v>
@@ -4008,9 +4108,15 @@
       <c r="B219" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C219" s="2"/>
-      <c r="D219" s="1"/>
-      <c r="E219" s="1"/>
+      <c r="C219" s="2">
+        <v>37.76</v>
+      </c>
+      <c r="D219" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
@@ -4022,8 +4128,8 @@
       <c r="C220" s="2">
         <v>37.69</v>
       </c>
-      <c r="D220" s="2" t="s">
-        <v>340</v>
+      <c r="D220" s="5">
+        <v>43188</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>339</v>
@@ -4039,8 +4145,8 @@
       <c r="C221" s="2">
         <v>37.700000000000003</v>
       </c>
-      <c r="D221" s="1" t="s">
-        <v>340</v>
+      <c r="D221" s="4">
+        <v>43188</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>339</v>
@@ -4056,8 +4162,8 @@
       <c r="C222" s="2">
         <v>37.729999999999997</v>
       </c>
-      <c r="D222" s="1" t="s">
-        <v>340</v>
+      <c r="D222" s="4">
+        <v>43188</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>339</v>
@@ -4070,9 +4176,15 @@
       <c r="B223" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C223" s="2"/>
-      <c r="D223" s="1"/>
-      <c r="E223" s="1"/>
+      <c r="C223" s="2">
+        <v>37.74</v>
+      </c>
+      <c r="D223" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
@@ -4081,9 +4193,15 @@
       <c r="B224" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C224" s="2"/>
-      <c r="D224" s="1"/>
-      <c r="E224" s="1"/>
+      <c r="C224" s="2">
+        <v>37.770000000000003</v>
+      </c>
+      <c r="D224" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
@@ -4092,9 +4210,15 @@
       <c r="B225" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C225" s="2"/>
-      <c r="D225" s="1"/>
-      <c r="E225" s="1"/>
+      <c r="C225" s="2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D225" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
@@ -4106,8 +4230,8 @@
       <c r="C226" s="2">
         <v>37.729999999999997</v>
       </c>
-      <c r="D226" s="1" t="s">
-        <v>340</v>
+      <c r="D226" s="4">
+        <v>43188</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>339</v>
@@ -4123,8 +4247,8 @@
       <c r="C227" s="2">
         <v>37.64</v>
       </c>
-      <c r="D227" s="1" t="s">
-        <v>340</v>
+      <c r="D227" s="4">
+        <v>43188</v>
       </c>
       <c r="E227" s="1" t="s">
         <v>339</v>
@@ -4140,8 +4264,8 @@
       <c r="C228" s="2">
         <v>37.71</v>
       </c>
-      <c r="D228" s="1" t="s">
-        <v>340</v>
+      <c r="D228" s="4">
+        <v>43188</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>339</v>
@@ -4157,8 +4281,8 @@
       <c r="C229" s="2">
         <v>37.71</v>
       </c>
-      <c r="D229" s="1" t="s">
-        <v>340</v>
+      <c r="D229" s="4">
+        <v>43188</v>
       </c>
       <c r="E229" s="1" t="s">
         <v>339</v>
@@ -4174,8 +4298,8 @@
       <c r="C230" s="2">
         <v>37.72</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>340</v>
+      <c r="D230" s="4">
+        <v>43188</v>
       </c>
       <c r="E230" s="1" t="s">
         <v>339</v>
@@ -4191,8 +4315,8 @@
       <c r="C231" s="2">
         <v>37.67</v>
       </c>
-      <c r="D231" s="1" t="s">
-        <v>340</v>
+      <c r="D231" s="4">
+        <v>43188</v>
       </c>
       <c r="E231" s="1" t="s">
         <v>339</v>
@@ -4845,9 +4969,15 @@
       <c r="B288" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C288" s="2"/>
-      <c r="D288" s="1"/>
-      <c r="E288" s="1"/>
+      <c r="C288" s="2">
+        <v>38.119999999999997</v>
+      </c>
+      <c r="D288" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
@@ -4924,9 +5054,15 @@
       <c r="B293" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C293" s="2"/>
-      <c r="D293" s="1"/>
-      <c r="E293" s="1"/>
+      <c r="C293" s="2">
+        <v>38.1</v>
+      </c>
+      <c r="D293" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
@@ -4969,9 +5105,15 @@
       <c r="B296" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C296" s="2"/>
-      <c r="D296" s="1"/>
-      <c r="E296" s="1"/>
+      <c r="C296" s="2">
+        <v>38.090000000000003</v>
+      </c>
+      <c r="D296" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
@@ -5015,10 +5157,14 @@
         <v>296</v>
       </c>
       <c r="C299" s="2">
-        <v>37.9</v>
-      </c>
-      <c r="D299" s="1"/>
-      <c r="E299" s="1"/>
+        <v>37.83</v>
+      </c>
+      <c r="D299" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E299" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
@@ -5044,9 +5190,15 @@
       <c r="B301" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C301" s="2"/>
-      <c r="D301" s="1"/>
-      <c r="E301" s="1"/>
+      <c r="C301" s="2">
+        <v>38.020000000000003</v>
+      </c>
+      <c r="D301" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
@@ -5055,9 +5207,15 @@
       <c r="B302" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C302" s="2"/>
-      <c r="D302" s="1"/>
-      <c r="E302" s="1"/>
+      <c r="C302" s="2">
+        <v>37.979999999999997</v>
+      </c>
+      <c r="D302" s="4">
+        <v>43192</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
@@ -5169,10 +5327,10 @@
         <v>306</v>
       </c>
       <c r="C309" s="2">
-        <v>37.64</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="D309" s="4">
-        <v>43187</v>
+        <v>43192</v>
       </c>
       <c r="E309" s="1" t="s">
         <v>339</v>

</xml_diff>